<commit_message>
Added a bunch of models
</commit_message>
<xml_diff>
--- a/Consumer/Costco Wholesale.xlsx
+++ b/Consumer/Costco Wholesale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Consumer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7590B4AB-C788-BE4F-930F-9A45CC0220CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E265AA-8C2A-A341-AF40-837634BF4417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="163">
   <si>
     <t>INCOME STATEMENT (in mln.)</t>
   </si>
@@ -551,16 +551,26 @@
   <si>
     <t>Buy/Sell</t>
   </si>
+  <si>
+    <t>Forward P/S</t>
+  </si>
+  <si>
+    <t>Forward P/E</t>
+  </si>
+  <si>
+    <t>Forward P/FCF</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="#,###,,;\(#,###,,\);\ \-\ \-"/>
     <numFmt numFmtId="165" formatCode="#.00%;\ \-#.00%;\ \-\ \-"/>
     <numFmt numFmtId="166" formatCode="#,##0.00_);\(#,##0.00\);\-\ \-"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -729,7 +739,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -893,12 +903,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -950,12 +969,6 @@
     <xf numFmtId="10" fontId="12" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1014,6 +1027,14 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="39" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1026,14 +1047,20 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="39" fontId="11" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="1" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2529,12 +2556,10 @@
     <v>1</v>
     <v>Powered by Refinitiv</v>
     <v>564.75</v>
-    <v>406.51010000000002</v>
-    <v>0.79379999999999995</v>
-    <v>1.73</v>
-    <v>3.467E-3</v>
-    <v>0.01</v>
-    <v>1.997E-5</v>
+    <v>443.2</v>
+    <v>0.79259999999999997</v>
+    <v>3.53</v>
+    <v>6.9479999999999993E-3</v>
     <v>USD</v>
     <v>Costco Wholesale Corporation is a global retailer with warehouse club operations in eight countries. The Company operates an international chain of membership warehouses, mainly under the Costco Wholesale name. The Company's warehouses are designed to help small- to medium-sized businesses reduce costs in purchasing for resale and for everyday business use. The Company offers merchandise in various categories, which include groceries, candy, appliances, television and media, automotive supplies, tires, toys, hardware, sporting goods, jewelry, watches, cameras, books, housewares, apparel, health and beauty aids, furniture, office supplies and office equipment. Members can also shop for private label Kirkland Signature products. It operates approximately 838 warehouses worldwide. It also operates self-service gasoline stations. The Company operates e-commerce websites in the United States, Canada, Mexico, United Kingdom, Korea, Taiwan, Japan, and Australia.</v>
     <v>304000</v>
@@ -2542,25 +2567,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>999 Lake Dr, ISSAQUAH, WA, 98027- US</v>
-    <v>501.74</v>
+    <v>513.86500000000001</v>
     <v>Diversified Retail</v>
     <v>Stock</v>
-    <v>45055.998605647655</v>
+    <v>45077.999619930466</v>
     <v>0</v>
-    <v>496.39</v>
-    <v>222091951728</v>
+    <v>504.95</v>
+    <v>226734646320</v>
     <v>COSTCO WHOLESALE CORPORATION</v>
     <v>COSTCO WHOLESALE CORPORATION</v>
-    <v>496.96</v>
-    <v>36.7988</v>
-    <v>499.06</v>
-    <v>500.79</v>
-    <v>500.8</v>
-    <v>443483200</v>
+    <v>508.86</v>
+    <v>37.899799999999999</v>
+    <v>508.03</v>
+    <v>511.56</v>
+    <v>443222000</v>
     <v>COST</v>
     <v>COSTCO WHOLESALE CORPORATION (XNAS:COST)</v>
-    <v>1571815</v>
-    <v>1741178</v>
+    <v>101</v>
+    <v>1835110</v>
     <v>1987</v>
   </rv>
   <rv s="2">
@@ -2592,8 +2616,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -2614,7 +2636,6 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -2631,7 +2652,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="1">
-    <a count="45">
+    <a count="42">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -2642,16 +2663,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -2717,19 +2735,13 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
     <spb s="4">
-      <v>at close</v>
+      <v>Delayed 15 minutes</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
-      <v>from close</v>
-      <v>from close</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
@@ -2774,9 +2786,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -2784,9 +2793,6 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
-    <k n="Price (Extended hours)" t="s"/>
-    <k n="Change (Extended hours)" t="s"/>
-    <k n="Change % (Extended hours)" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -3148,10 +3154,10 @@
   <dimension ref="A1:AV118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK89" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AN103" sqref="AN103"/>
+      <selection pane="bottomRight" activeCell="AO122" sqref="AO122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3543,20 +3549,20 @@
       <c r="AM3" s="1">
         <v>226954000000</v>
       </c>
-      <c r="AN3" s="1">
-        <v>243000000000</v>
-      </c>
-      <c r="AO3" s="1">
-        <v>259200000000</v>
-      </c>
-      <c r="AP3" s="1">
-        <v>277000000000</v>
-      </c>
-      <c r="AQ3" s="1">
-        <v>297500000000</v>
-      </c>
-      <c r="AR3" s="1">
-        <v>313600000000</v>
+      <c r="AN3" s="70">
+        <v>242400000000</v>
+      </c>
+      <c r="AO3" s="70">
+        <v>254900000000</v>
+      </c>
+      <c r="AP3" s="70">
+        <v>272500000000</v>
+      </c>
+      <c r="AQ3" s="70">
+        <v>294300000000</v>
+      </c>
+      <c r="AR3" s="70">
+        <v>314900000000</v>
       </c>
       <c r="AS3" s="18" t="s">
         <v>109</v>
@@ -3726,23 +3732,23 @@
       </c>
       <c r="AN4" s="16">
         <f t="shared" si="0"/>
-        <v>7.0701551856323208E-2</v>
+        <v>6.8057844320875693E-2</v>
       </c>
       <c r="AO4" s="16">
         <f t="shared" si="0"/>
-        <v>6.6666666666666652E-2</v>
+        <v>5.156765676567665E-2</v>
       </c>
       <c r="AP4" s="16">
         <f t="shared" si="0"/>
-        <v>6.8672839506172867E-2</v>
+        <v>6.9046684974499728E-2</v>
       </c>
       <c r="AQ4" s="16">
         <f t="shared" si="0"/>
-        <v>7.400722021660644E-2</v>
+        <v>8.0000000000000071E-2</v>
       </c>
       <c r="AR4" s="16">
         <f t="shared" si="0"/>
-        <v>5.4117647058823604E-2</v>
+        <v>6.9996602106693784E-2</v>
       </c>
       <c r="AS4" s="17">
         <f>(AM4+AL4+AK4)/3</f>
@@ -5364,20 +5370,20 @@
         <f>(AM35+AL35+AK35+AJ35+AI35)/5</f>
         <v>1.726904036736459E-3</v>
       </c>
-      <c r="AT16" s="29">
+      <c r="AT16" s="71">
         <f>AU101/AM3</f>
-        <v>0.97857694390933847</v>
-      </c>
-      <c r="AU16" s="29">
+        <v>0.99903348837209305</v>
+      </c>
+      <c r="AU16" s="71">
         <f>AU101/AM28</f>
-        <v>38.003414053388092</v>
-      </c>
-      <c r="AV16" s="30">
+        <v>38.797851868583159</v>
+      </c>
+      <c r="AV16" s="72">
         <f>AU101/AM106</f>
-        <v>63.436718574121677</v>
+        <v>64.762823856041138</v>
       </c>
     </row>
-    <row r="17" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>12</v>
       </c>
@@ -5496,7 +5502,7 @@
         <v>158000000</v>
       </c>
     </row>
-    <row r="18" spans="1:45" ht="20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:48" ht="20" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
@@ -5617,8 +5623,17 @@
       <c r="AS18" s="18" t="s">
         <v>125</v>
       </c>
+      <c r="AT18" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="AU18" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="AV18" s="19" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="19" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>14</v>
       </c>
@@ -5736,12 +5751,39 @@
       <c r="AM19" s="10">
         <v>9827000000</v>
       </c>
-      <c r="AS19" s="31">
+      <c r="AN19" s="68">
+        <v>10540000000</v>
+      </c>
+      <c r="AO19" s="68">
+        <v>11298000000</v>
+      </c>
+      <c r="AP19" s="68">
+        <v>12473000000</v>
+      </c>
+      <c r="AQ19" s="68">
+        <v>13849000000</v>
+      </c>
+      <c r="AR19" s="68">
+        <v>15193000000</v>
+      </c>
+      <c r="AS19" s="29">
         <f>AM40-AM56-AM61</f>
         <v>2010000000</v>
       </c>
+      <c r="AT19" s="71">
+        <f>AU101/AN3</f>
+        <v>0.93537395346534657</v>
+      </c>
+      <c r="AU19" s="71">
+        <f>AU101/AN28</f>
+        <v>35.109112158563022</v>
+      </c>
+      <c r="AV19" s="72">
+        <f>AU101/AN105</f>
+        <v>43.974912009309541</v>
+      </c>
     </row>
-    <row r="20" spans="1:45" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:48" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>101</v>
       </c>
@@ -5894,8 +5936,28 @@
         <f t="shared" ref="AM20" si="5">(AM19/AL19)-1</f>
         <v>0.14801401869158881</v>
       </c>
+      <c r="AN20" s="16">
+        <f t="shared" ref="AN20" si="6">(AN19/AM19)-1</f>
+        <v>7.2555205047318605E-2</v>
+      </c>
+      <c r="AO20" s="16">
+        <f t="shared" ref="AO20" si="7">(AO19/AN19)-1</f>
+        <v>7.1916508538899526E-2</v>
+      </c>
+      <c r="AP20" s="16">
+        <f t="shared" ref="AP20" si="8">(AP19/AO19)-1</f>
+        <v>0.10400070808992745</v>
+      </c>
+      <c r="AQ20" s="16">
+        <f t="shared" ref="AQ20" si="9">(AQ19/AP19)-1</f>
+        <v>0.11031828750100225</v>
+      </c>
+      <c r="AR20" s="16">
+        <f t="shared" ref="AR20" si="10">(AR19/AQ19)-1</f>
+        <v>9.7046718174597535E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
@@ -6013,8 +6075,28 @@
       <c r="AM21" s="2">
         <v>4.3299999999999998E-2</v>
       </c>
+      <c r="AN21" s="69">
+        <f>AN19/AN3</f>
+        <v>4.3481848184818483E-2</v>
+      </c>
+      <c r="AO21" s="69">
+        <f t="shared" ref="AO21:AR21" si="11">AO19/AO3</f>
+        <v>4.4323264025107882E-2</v>
+      </c>
+      <c r="AP21" s="69">
+        <f t="shared" si="11"/>
+        <v>4.5772477064220184E-2</v>
+      </c>
+      <c r="AQ21" s="69">
+        <f t="shared" si="11"/>
+        <v>4.7057424396873937E-2</v>
+      </c>
+      <c r="AR21" s="69">
+        <f t="shared" si="11"/>
+        <v>4.8247062559542711E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>16</v>
       </c>
@@ -6133,7 +6215,7 @@
         <v>7793000000</v>
       </c>
     </row>
-    <row r="23" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
@@ -6252,7 +6334,7 @@
         <v>3.4299999999999997E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
@@ -6371,7 +6453,7 @@
         <v>47000000</v>
       </c>
     </row>
-    <row r="25" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>19</v>
       </c>
@@ -6490,7 +6572,7 @@
         <v>7840000000</v>
       </c>
     </row>
-    <row r="26" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>20</v>
       </c>
@@ -6609,7 +6691,7 @@
         <v>3.4500000000000003E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>21</v>
       </c>
@@ -6728,7 +6810,7 @@
         <v>1925000000</v>
       </c>
     </row>
-    <row r="28" spans="1:45" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:48" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>22</v>
       </c>
@@ -6846,8 +6928,23 @@
       <c r="AM28" s="11">
         <v>5844000000</v>
       </c>
+      <c r="AN28" s="65">
+        <v>6458000000</v>
+      </c>
+      <c r="AO28" s="65">
+        <v>6912000000</v>
+      </c>
+      <c r="AP28" s="65">
+        <v>7750000000</v>
+      </c>
+      <c r="AQ28" s="65">
+        <v>8243000000</v>
+      </c>
+      <c r="AR28" s="65">
+        <v>8999000000</v>
+      </c>
     </row>
-    <row r="29" spans="1:45" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:48" ht="20" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>102</v>
       </c>
@@ -6865,143 +6962,163 @@
         <v>0.29331514324693053</v>
       </c>
       <c r="F29" s="15">
-        <f t="shared" ref="F29:AK29" si="6">(F28/E28)-1</f>
+        <f t="shared" ref="F29:AK29" si="12">(F28/E28)-1</f>
         <v>0.23417721518987333</v>
       </c>
       <c r="G29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>7.1794871794871762E-2</v>
       </c>
       <c r="H29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>6.9377990430621983E-2</v>
       </c>
       <c r="I29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>-3.7285607755406458E-2</v>
       </c>
       <c r="J29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.72889233152594879</v>
       </c>
       <c r="K29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>-1.5035842293906811</v>
       </c>
       <c r="L29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>-2.1903914590747329</v>
       </c>
       <c r="M29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.85949177877428995</v>
       </c>
       <c r="N29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.25482315112540199</v>
       </c>
       <c r="O29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.47277386290839196</v>
       </c>
       <c r="P29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>-0.13592866463679865</v>
       </c>
       <c r="Q29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.58932041278630765</v>
       </c>
       <c r="R29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>-4.6478112622478585E-2</v>
       </c>
       <c r="S29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.16259058046235686</v>
       </c>
       <c r="T29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3.0025014893218849E-2</v>
       </c>
       <c r="U29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.22384604715672674</v>
       </c>
       <c r="V29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.20478290285621026</v>
       </c>
       <c r="W29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3.7741794689452934E-2</v>
       </c>
       <c r="X29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>-1.853038618945535E-2</v>
       </c>
       <c r="Y29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.18466768627190211</v>
       </c>
       <c r="Z29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>-0.15336490674150738</v>
       </c>
       <c r="AA29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.19981583793738489</v>
       </c>
       <c r="AB29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.12202609363008432</v>
       </c>
       <c r="AC29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.16894664842681251</v>
       </c>
       <c r="AD29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.19309537741369232</v>
       </c>
       <c r="AE29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9.3182932810200736E-3</v>
       </c>
       <c r="AF29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.15500485908649164</v>
       </c>
       <c r="AG29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>-1.13588557004628E-2</v>
       </c>
       <c r="AH29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.1399999999999999</v>
       </c>
       <c r="AI29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.16983949234789097</v>
       </c>
       <c r="AJ29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>0.16751754945756225</v>
       </c>
       <c r="AK29" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>9.3741459415140671E-2</v>
       </c>
       <c r="AL29" s="15">
-        <f t="shared" ref="AL29" si="7">(AL28/AK28)-1</f>
+        <f t="shared" ref="AL29" si="13">(AL28/AK28)-1</f>
         <v>0.25112443778110949</v>
       </c>
       <c r="AM29" s="15">
-        <f t="shared" ref="AM29" si="8">(AM28/AL28)-1</f>
+        <f t="shared" ref="AM29" si="14">(AM28/AL28)-1</f>
         <v>0.16716596764529656</v>
       </c>
+      <c r="AN29" s="16">
+        <f t="shared" ref="AN29" si="15">(AN28/AM28)-1</f>
+        <v>0.10506502395619433</v>
+      </c>
+      <c r="AO29" s="16">
+        <f t="shared" ref="AO29" si="16">(AO28/AN28)-1</f>
+        <v>7.0300402601424672E-2</v>
+      </c>
+      <c r="AP29" s="16">
+        <f t="shared" ref="AP29" si="17">(AP28/AO28)-1</f>
+        <v>0.12123842592592582</v>
+      </c>
+      <c r="AQ29" s="16">
+        <f t="shared" ref="AQ29" si="18">(AQ28/AP28)-1</f>
+        <v>6.3612903225806372E-2</v>
+      </c>
+      <c r="AR29" s="16">
+        <f t="shared" ref="AR29" si="19">(AR28/AQ28)-1</f>
+        <v>9.1714181729952715E-2</v>
+      </c>
     </row>
-    <row r="30" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
@@ -7119,8 +7236,28 @@
       <c r="AM30" s="2">
         <v>2.5700000000000001E-2</v>
       </c>
+      <c r="AN30" s="66">
+        <f>AN28/AN3</f>
+        <v>2.6641914191419144E-2</v>
+      </c>
+      <c r="AO30" s="66">
+        <f t="shared" ref="AO30:AR30" si="20">AO28/AO3</f>
+        <v>2.7116516280894468E-2</v>
+      </c>
+      <c r="AP30" s="66">
+        <f t="shared" si="20"/>
+        <v>2.8440366972477066E-2</v>
+      </c>
+      <c r="AQ30" s="66">
+        <f t="shared" si="20"/>
+        <v>2.8008834522595991E-2</v>
+      </c>
+      <c r="AR30" s="66">
+        <f t="shared" si="20"/>
+        <v>2.857732613528104E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>24</v>
       </c>
@@ -7238,8 +7375,23 @@
       <c r="AM31" s="12">
         <v>13.17</v>
       </c>
+      <c r="AN31" s="67">
+        <v>14.56</v>
+      </c>
+      <c r="AO31" s="67">
+        <v>15.59</v>
+      </c>
+      <c r="AP31" s="67">
+        <v>17.48</v>
+      </c>
+      <c r="AQ31" s="67">
+        <v>18.59</v>
+      </c>
+      <c r="AR31" s="67">
+        <v>20.29</v>
+      </c>
     </row>
-    <row r="32" spans="1:45" ht="19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:48" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>25</v>
       </c>
@@ -7606,147 +7758,147 @@
         <v>2.4347822566351613E-2</v>
       </c>
       <c r="D35" s="22">
-        <f t="shared" ref="D35:AK35" si="9">(D34-C34)/C34</f>
+        <f t="shared" ref="D35:AK35" si="21">(D34-C34)/C34</f>
         <v>6.6699005206619699E-2</v>
       </c>
       <c r="E35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-1.5955864971260298E-2</v>
       </c>
       <c r="F35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>3.0205904782222584E-2</v>
       </c>
       <c r="G35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>2.4161893816647198E-2</v>
       </c>
       <c r="H35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.23343315771857359</v>
       </c>
       <c r="I35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-9.1778873974645792E-2</v>
       </c>
       <c r="J35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>0.83262586886233414</v>
       </c>
       <c r="K35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-3.1568790322580642E-2</v>
       </c>
       <c r="L35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-8.9700647750676613E-2</v>
       </c>
       <c r="M35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>3.6438038842189512E-2</v>
       </c>
       <c r="N35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>4.8550853792581346E-2</v>
       </c>
       <c r="O35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>5.404403947833452E-2</v>
       </c>
       <c r="P35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>1.3049151927677768E-2</v>
       </c>
       <c r="Q35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>4.1759853254189891E-2</v>
       </c>
       <c r="R35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>1.8918015626280906E-4</v>
       </c>
       <c r="S35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>7.2190102705395028E-3</v>
       </c>
       <c r="T35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>1.3353864900618034E-4</v>
       </c>
       <c r="U35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>6.5362613336226285E-3</v>
       </c>
       <c r="V35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>1.9848318717238148E-2</v>
       </c>
       <c r="W35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-2.3766601969372098E-2</v>
       </c>
       <c r="X35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-4.7258093729246511E-2</v>
       </c>
       <c r="Y35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-2.9282778422387853E-2</v>
       </c>
       <c r="Z35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-8.5224203133441381E-3</v>
       </c>
       <c r="AA35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>1.2523441721496456E-2</v>
       </c>
       <c r="AB35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-6.448864273381618E-3</v>
       </c>
       <c r="AC35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-8.3977666138562029E-3</v>
       </c>
       <c r="AD35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>2.5923304345055339E-3</v>
       </c>
       <c r="AE35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>4.4788791224756649E-3</v>
       </c>
       <c r="AF35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>5.2205159496932104E-4</v>
       </c>
       <c r="AG35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-3.2820137514795039E-3</v>
       </c>
       <c r="AH35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>-7.3878843229547913E-4</v>
       </c>
       <c r="AI35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>2.0343042203307955E-3</v>
       </c>
       <c r="AJ35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>2.4647265715178101E-3</v>
       </c>
       <c r="AK35" s="22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="21"/>
         <v>2.2080587370716808E-3</v>
       </c>
       <c r="AL35" s="22">
-        <f t="shared" ref="AL35" si="10">(AL34-AK34)/AK34</f>
+        <f t="shared" ref="AL35" si="22">(AL34-AK34)/AK34</f>
         <v>1.0024757772566406E-3</v>
       </c>
       <c r="AM35" s="22">
-        <f t="shared" ref="AM35" si="11">(AM34-AL34)/AL34</f>
+        <f t="shared" ref="AM35" si="23">(AM34-AL34)/AL34</f>
         <v>9.2495487750536749E-4</v>
       </c>
     </row>
@@ -12991,155 +13143,155 @@
         <v>104</v>
       </c>
       <c r="B80" s="15" t="e">
-        <f t="shared" ref="B80:AM80" si="12">B79/B3</f>
+        <f t="shared" ref="B80:AM80" si="24">B79/B3</f>
         <v>#VALUE!</v>
       </c>
       <c r="C80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="D80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="E80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="F80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="G80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="H80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="I80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="J80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="K80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="L80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="M80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="N80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="O80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="P80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="Q80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="R80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="S80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="T80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="U80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="V80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="W80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="X80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="Y80" s="15" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>#VALUE!</v>
       </c>
       <c r="Z80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>2.5342331494497493E-3</v>
       </c>
       <c r="AA80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>2.437584994739948E-3</v>
       </c>
       <c r="AB80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>2.3280661305741437E-3</v>
       </c>
       <c r="AC80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>2.4309793518060866E-3</v>
       </c>
       <c r="AD80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>2.7102590437064933E-3</v>
       </c>
       <c r="AE80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>2.9030539772727272E-3</v>
       </c>
       <c r="AF80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>3.390734860024613E-3</v>
       </c>
       <c r="AG80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>3.8662724584944282E-3</v>
       </c>
       <c r="AH80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>3.9837240844797523E-3</v>
       </c>
       <c r="AI80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>3.8424591738712775E-3</v>
       </c>
       <c r="AJ80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>3.8964525909772566E-3</v>
       </c>
       <c r="AK80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>3.7118990651291367E-3</v>
       </c>
       <c r="AL80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>3.3940866334233317E-3</v>
       </c>
       <c r="AM80" s="15">
-        <f t="shared" si="12"/>
+        <f t="shared" si="24"/>
         <v>3.1900737594402389E-3</v>
       </c>
     </row>
@@ -13499,10 +13651,10 @@
       <c r="AM83" s="1">
         <v>-4003000000</v>
       </c>
-      <c r="AT83" s="57" t="s">
+      <c r="AT83" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="AU83" s="58"/>
+      <c r="AU83" s="60"/>
     </row>
     <row r="84" spans="1:47" ht="19" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
@@ -13622,10 +13774,10 @@
       <c r="AM84" s="1">
         <v>1891000000</v>
       </c>
-      <c r="AT84" s="59" t="s">
+      <c r="AT84" s="61" t="s">
         <v>127</v>
       </c>
-      <c r="AU84" s="60"/>
+      <c r="AU84" s="62"/>
     </row>
     <row r="85" spans="1:47" ht="20" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
@@ -14123,10 +14275,10 @@
       <c r="AM88" s="1">
         <v>-3891000000</v>
       </c>
-      <c r="AT88" s="32" t="s">
+      <c r="AT88" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="AU88" s="33">
+      <c r="AU88" s="31">
         <f>AU85/(AU86+AU87)</f>
         <v>1.7479809713463877E-2</v>
       </c>
@@ -14136,155 +14288,155 @@
         <v>105</v>
       </c>
       <c r="B89" s="15" t="e">
-        <f t="shared" ref="B89:AM89" si="13">(-1*B88)/B3</f>
+        <f t="shared" ref="B89:AM89" si="25">(-1*B88)/B3</f>
         <v>#VALUE!</v>
       </c>
       <c r="C89" s="15" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>#VALUE!</v>
       </c>
       <c r="D89" s="15" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>#VALUE!</v>
       </c>
       <c r="E89" s="15" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>#VALUE!</v>
       </c>
       <c r="F89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>3.2685872847465929E-2</v>
       </c>
       <c r="G89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>3.0587345124373402E-2</v>
       </c>
       <c r="H89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>3.8950606992922202E-2</v>
       </c>
       <c r="I89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>5.9328980082511404E-2</v>
       </c>
       <c r="J89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>3.5170607138379516E-2</v>
       </c>
       <c r="K89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.8797495236823904E-2</v>
       </c>
       <c r="L89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.9632690900764553E-2</v>
       </c>
       <c r="M89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.5901413129583727E-2</v>
       </c>
       <c r="N89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.5298979629155543E-2</v>
       </c>
       <c r="O89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.3564167961137045E-2</v>
       </c>
       <c r="P89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.869682400932401E-2</v>
       </c>
       <c r="Q89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>3.8192068621679141E-2</v>
       </c>
       <c r="R89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>4.1599777590258617E-2</v>
       </c>
       <c r="S89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.6794067121420628E-2</v>
       </c>
       <c r="T89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.9054048235171563E-2</v>
       </c>
       <c r="U89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.4667722313629587E-2</v>
       </c>
       <c r="V89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.8804698451473562E-2</v>
       </c>
       <c r="W89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.0158641152906158E-2</v>
       </c>
       <c r="X89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.1517013429548423E-2</v>
       </c>
       <c r="Y89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.205442046978727E-2</v>
       </c>
       <c r="Z89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.7501610148133628E-2</v>
       </c>
       <c r="AA89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.3535011418161292E-2</v>
       </c>
       <c r="AB89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.4508238205027273E-2</v>
       </c>
       <c r="AC89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.4928835853414972E-2</v>
       </c>
       <c r="AD89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.9808665221195176E-2</v>
       </c>
       <c r="AE89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.7693536931818181E-2</v>
       </c>
       <c r="AF89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.0593981015327154E-2</v>
       </c>
       <c r="AG89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.231319333889268E-2</v>
       </c>
       <c r="AH89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.9391590776981205E-2</v>
       </c>
       <c r="AI89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>2.0971068542690853E-2</v>
       </c>
       <c r="AJ89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.9632882130671957E-2</v>
       </c>
       <c r="AK89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.685046263814681E-2</v>
       </c>
       <c r="AL89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.8312756151463029E-2</v>
       </c>
       <c r="AM89" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="25"/>
         <v>1.7144443367378411E-2</v>
       </c>
       <c r="AT89" s="23" t="s">
@@ -14539,10 +14691,10 @@
       <c r="AM91" s="1">
         <v>-1121000000</v>
       </c>
-      <c r="AT91" s="32" t="s">
+      <c r="AT91" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="AU91" s="33">
+      <c r="AU91" s="31">
         <f>AU89/AU90</f>
         <v>0.24553571428571427</v>
       </c>
@@ -14665,10 +14817,10 @@
       <c r="AM92" s="1">
         <v>1145000000</v>
       </c>
-      <c r="AT92" s="34" t="s">
+      <c r="AT92" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="AU92" s="35">
+      <c r="AU92" s="33">
         <f>AU88*(1-AU91)</f>
         <v>1.3187892149890157E-2</v>
       </c>
@@ -14791,10 +14943,10 @@
       <c r="AM93" s="1">
         <v>-48000000</v>
       </c>
-      <c r="AT93" s="59" t="s">
+      <c r="AT93" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="AU93" s="60"/>
+      <c r="AU93" s="62"/>
     </row>
     <row r="94" spans="1:47" ht="20" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
@@ -14917,7 +15069,7 @@
       <c r="AT94" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="AU94" s="36">
+      <c r="AU94" s="34">
         <v>4.095E-2</v>
       </c>
     </row>
@@ -15039,12 +15191,12 @@
       <c r="AM95" s="1">
         <v>-800000000</v>
       </c>
-      <c r="AT95" s="56" t="s">
+      <c r="AT95" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="AU95" s="63" cm="1">
+      <c r="AU95" s="55" cm="1">
         <f t="array" ref="AU95">_FV(A1,"Beta")</f>
-        <v>0.79379999999999995</v>
+        <v>0.79259999999999997</v>
       </c>
     </row>
     <row r="96" spans="1:47" ht="20" x14ac:dyDescent="0.25">
@@ -15168,7 +15320,7 @@
       <c r="AT96" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="AU96" s="36">
+      <c r="AU96" s="34">
         <v>8.4000000000000005E-2</v>
       </c>
     </row>
@@ -15290,12 +15442,12 @@
       <c r="AM97" s="1">
         <v>-439000000</v>
       </c>
-      <c r="AT97" s="34" t="s">
+      <c r="AT97" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="AU97" s="35">
+      <c r="AU97" s="33">
         <f>(AU94)+((AU95)*(AU96-AU94))</f>
-        <v>7.5123090000000003E-2</v>
+        <v>7.5071429999999995E-2</v>
       </c>
     </row>
     <row r="98" spans="1:47" ht="19" x14ac:dyDescent="0.25">
@@ -15416,10 +15568,10 @@
       <c r="AM98" s="1">
         <v>-1498000000</v>
       </c>
-      <c r="AT98" s="59" t="s">
+      <c r="AT98" s="61" t="s">
         <v>139</v>
       </c>
-      <c r="AU98" s="60"/>
+      <c r="AU98" s="62"/>
     </row>
     <row r="99" spans="1:47" ht="20" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
@@ -15665,12 +15817,12 @@
       <c r="AM100" s="10">
         <v>-4283000000</v>
       </c>
-      <c r="AT100" s="32" t="s">
+      <c r="AT100" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="AU100" s="33">
+      <c r="AU100" s="31">
         <f>AU99/AU103</f>
-        <v>3.9107700342260063E-2</v>
+        <v>3.8337618054784472E-2</v>
       </c>
     </row>
     <row r="101" spans="1:47" ht="20" x14ac:dyDescent="0.25">
@@ -15791,12 +15943,12 @@
       <c r="AM101" s="1">
         <v>-249000000</v>
       </c>
-      <c r="AT101" s="56" t="s">
+      <c r="AT101" s="54" t="s">
         <v>142</v>
       </c>
-      <c r="AU101" s="49" cm="1">
+      <c r="AU101" s="47" cm="1">
         <f t="array" ref="AU101">_FV(A1,"Market cap",TRUE)</f>
-        <v>222091951728</v>
+        <v>226734646320</v>
       </c>
     </row>
     <row r="102" spans="1:47" ht="20" x14ac:dyDescent="0.25">
@@ -15917,12 +16069,12 @@
       <c r="AM102" s="10">
         <v>-1055000000</v>
       </c>
-      <c r="AT102" s="32" t="s">
+      <c r="AT102" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="AU102" s="33">
+      <c r="AU102" s="31">
         <f>AU101/AU103</f>
-        <v>0.96089229965773992</v>
+        <v>0.96166238194521558</v>
       </c>
     </row>
     <row r="103" spans="1:47" ht="20" x14ac:dyDescent="0.25">
@@ -16043,12 +16195,12 @@
       <c r="AM103" s="1">
         <v>11258000000</v>
       </c>
-      <c r="AT103" s="34" t="s">
+      <c r="AT103" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="AU103" s="37">
+      <c r="AU103" s="35">
         <f>AU99+AU101</f>
-        <v>231130951728</v>
+        <v>235773646320</v>
       </c>
     </row>
     <row r="104" spans="1:47" ht="20" thickBot="1" x14ac:dyDescent="0.3">
@@ -16169,10 +16321,10 @@
       <c r="AM104" s="11">
         <v>10203000000</v>
       </c>
-      <c r="AT104" s="59" t="s">
+      <c r="AT104" s="61" t="s">
         <v>145</v>
       </c>
-      <c r="AU104" s="60"/>
+      <c r="AU104" s="62"/>
     </row>
     <row r="105" spans="1:47" ht="21" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
@@ -16200,145 +16352,155 @@
         <v>-4.2895442359249358E-2</v>
       </c>
       <c r="H105" s="15">
-        <f t="shared" ref="H105:AK105" si="14">(H106/G106)-1</f>
+        <f t="shared" ref="H105:AK105" si="26">(H106/G106)-1</f>
         <v>-0.4509803921568627</v>
       </c>
       <c r="I105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>13.244897959183673</v>
       </c>
       <c r="J105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.15042979942693413</v>
       </c>
       <c r="K105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-4.3844856661045539E-2</v>
       </c>
       <c r="L105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>0.11199294532627868</v>
       </c>
       <c r="M105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.68120539254559875</v>
       </c>
       <c r="N105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-1.4577114427860698</v>
       </c>
       <c r="O105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>3.5027173913043477</v>
       </c>
       <c r="P105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-7.664453832226914E-2</v>
       </c>
       <c r="Q105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-2.0330915032679737</v>
       </c>
       <c r="R105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>1.625446815510271</v>
       </c>
       <c r="S105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.95093328449634451</v>
       </c>
       <c r="T105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-35.207985463117573</v>
       </c>
       <c r="U105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>1.000110545939016</v>
       </c>
       <c r="V105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.43456293341123764</v>
       </c>
       <c r="W105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.21964313370045674</v>
       </c>
       <c r="X105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>0.12360363936276997</v>
       </c>
       <c r="Y105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.1637500814385302</v>
       </c>
       <c r="Z105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>0.45775118507207391</v>
       </c>
       <c r="AA105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>1.0486935866983371</v>
       </c>
       <c r="AB105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>0.10608695652173905</v>
       </c>
       <c r="AC105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.1734800838574424</v>
       </c>
       <c r="AD105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.14140773620798985</v>
       </c>
       <c r="AE105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>0.47045790251107822</v>
       </c>
       <c r="AF105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-4.9723756906077332E-2</v>
       </c>
       <c r="AG105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.66014799154334036</v>
       </c>
       <c r="AH105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>5.5692068429237951</v>
       </c>
       <c r="AI105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>-0.3359375</v>
       </c>
       <c r="AJ105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>0.19714795008912667</v>
       </c>
       <c r="AK105" s="15">
-        <f t="shared" si="14"/>
+        <f t="shared" si="26"/>
         <v>0.8019654556283502</v>
       </c>
       <c r="AL105" s="15">
-        <f t="shared" ref="AL105" si="15">(AL106/AK106)-1</f>
+        <f t="shared" ref="AL105" si="27">(AL106/AK106)-1</f>
         <v>-0.11254338125929597</v>
       </c>
       <c r="AM105" s="15">
-        <f t="shared" ref="AM105" si="16">(AM106/AL106)-1</f>
+        <f t="shared" ref="AM105" si="28">(AM106/AL106)-1</f>
         <v>-0.34804469273743022</v>
       </c>
-      <c r="AN105" s="15"/>
-      <c r="AO105" s="15"/>
-      <c r="AP105" s="15"/>
-      <c r="AQ105" s="15"/>
-      <c r="AR105" s="15"/>
+      <c r="AN105" s="63">
+        <v>5156000000</v>
+      </c>
+      <c r="AO105" s="63">
+        <v>5461000000</v>
+      </c>
+      <c r="AP105" s="63">
+        <v>6582000000</v>
+      </c>
+      <c r="AQ105" s="63">
+        <v>7726000000</v>
+      </c>
+      <c r="AR105" s="63">
+        <v>8253000000</v>
+      </c>
       <c r="AS105" s="15"/>
       <c r="AT105" s="25" t="s">
         <v>108</v>
       </c>
       <c r="AU105" s="26">
         <f>(AU100*AU92)+(AU102*AU97)</f>
-        <v>7.2700946841839323E-2</v>
+        <v>7.2698962562023697E-2</v>
       </c>
     </row>
     <row r="106" spans="1:47" ht="19" x14ac:dyDescent="0.25">
@@ -16459,35 +16621,35 @@
       <c r="AM106" s="1">
         <v>3501000000</v>
       </c>
-      <c r="AN106" s="38">
+      <c r="AN106" s="36">
         <f>AM106*(1+$AU$106)</f>
-        <v>3734982980.8982759</v>
-      </c>
-      <c r="AO106" s="38">
-        <f t="shared" ref="AO106:AR106" si="17">AN106*(1+$AU$106)</f>
-        <v>3984603789.6600313</v>
-      </c>
-      <c r="AP106" s="38">
-        <f t="shared" si="17"/>
-        <v>4250907552.1288176</v>
-      </c>
-      <c r="AQ106" s="38">
-        <f t="shared" si="17"/>
-        <v>4535009243.2370987</v>
-      </c>
-      <c r="AR106" s="38">
-        <f t="shared" si="17"/>
-        <v>4838098355.2433395</v>
-      </c>
-      <c r="AS106" s="39" t="s">
+        <v>3738135885.4750562</v>
+      </c>
+      <c r="AO106" s="36">
+        <f t="shared" ref="AO106:AR106" si="29">AN106*(1+$AU$106)</f>
+        <v>3991333875.5430965</v>
+      </c>
+      <c r="AP106" s="36">
+        <f t="shared" si="29"/>
+        <v>4261681916.9037075</v>
+      </c>
+      <c r="AQ106" s="36">
+        <f t="shared" si="29"/>
+        <v>4550341646.9745426</v>
+      </c>
+      <c r="AR106" s="36">
+        <f t="shared" si="29"/>
+        <v>4858553385.2405615</v>
+      </c>
+      <c r="AS106" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="AT106" s="40" t="s">
+      <c r="AT106" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="AU106" s="41">
+      <c r="AU106" s="39">
         <f>(SUM(AN4:AR4)/5)</f>
-        <v>6.6833185060918551E-2</v>
+        <v>6.7733757633549191E-2</v>
       </c>
     </row>
     <row r="107" spans="1:47" ht="19" x14ac:dyDescent="0.25">
@@ -16530,139 +16692,139 @@
       <c r="AK107" s="13"/>
       <c r="AL107" s="13"/>
       <c r="AM107" s="13"/>
-      <c r="AN107" s="39"/>
-      <c r="AO107" s="39"/>
-      <c r="AP107" s="39"/>
-      <c r="AQ107" s="39"/>
-      <c r="AR107" s="42">
-        <f>AR106*(1+AU107)/(AU108-AU107)</f>
-        <v>103961265812.33298</v>
-      </c>
-      <c r="AS107" s="43" t="s">
+      <c r="AN107" s="37"/>
+      <c r="AO107" s="37"/>
+      <c r="AP107" s="37"/>
+      <c r="AQ107" s="37"/>
+      <c r="AR107" s="64">
+        <f>AR105*(1+AU107)/(AU108-AU107)</f>
+        <v>177348196808.26828</v>
+      </c>
+      <c r="AS107" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="AT107" s="44" t="s">
+      <c r="AT107" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="AU107" s="45">
+      <c r="AU107" s="43">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="108" spans="1:47" ht="19" x14ac:dyDescent="0.25">
-      <c r="AN108" s="42">
-        <f t="shared" ref="AN108:AP108" si="18">AN107+AN106</f>
-        <v>3734982980.8982759</v>
-      </c>
-      <c r="AO108" s="42">
-        <f t="shared" si="18"/>
-        <v>3984603789.6600313</v>
-      </c>
-      <c r="AP108" s="42">
-        <f t="shared" si="18"/>
-        <v>4250907552.1288176</v>
-      </c>
-      <c r="AQ108" s="42">
+      <c r="AN108" s="40">
+        <f t="shared" ref="AN108:AP108" si="30">AN107+AN106</f>
+        <v>3738135885.4750562</v>
+      </c>
+      <c r="AO108" s="40">
+        <f t="shared" si="30"/>
+        <v>3991333875.5430965</v>
+      </c>
+      <c r="AP108" s="40">
+        <f t="shared" si="30"/>
+        <v>4261681916.9037075</v>
+      </c>
+      <c r="AQ108" s="40">
         <f>AQ107+AQ106</f>
-        <v>4535009243.2370987</v>
-      </c>
-      <c r="AR108" s="42">
-        <f>AR107+AR106</f>
-        <v>108799364167.57632</v>
-      </c>
-      <c r="AS108" s="43" t="s">
+        <v>4550341646.9745426</v>
+      </c>
+      <c r="AR108" s="64">
+        <f>AR107+AR105</f>
+        <v>185601196808.26828</v>
+      </c>
+      <c r="AS108" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="AT108" s="46" t="s">
+      <c r="AT108" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="AU108" s="47">
+      <c r="AU108" s="45">
         <f>AU105</f>
-        <v>7.2700946841839323E-2</v>
+        <v>7.2698962562023697E-2</v>
       </c>
     </row>
     <row r="109" spans="1:47" ht="19" x14ac:dyDescent="0.25">
-      <c r="AN109" s="61" t="s">
+      <c r="AN109" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="AO109" s="62"/>
+      <c r="AO109" s="58"/>
     </row>
     <row r="110" spans="1:47" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN110" s="48" t="s">
+      <c r="AN110" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="AO110" s="49">
+      <c r="AO110" s="47">
         <f>NPV(AU108,AN108,AO108,AP108,AQ108,AR108)</f>
-        <v>90414289904.14418</v>
+        <v>144517384699.57388</v>
       </c>
     </row>
     <row r="111" spans="1:47" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN111" s="48" t="s">
+      <c r="AN111" s="46" t="s">
         <v>153</v>
       </c>
-      <c r="AO111" s="49">
+      <c r="AO111" s="47">
         <f>AM40</f>
         <v>11049000000</v>
       </c>
     </row>
     <row r="112" spans="1:47" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN112" s="48" t="s">
+      <c r="AN112" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="AO112" s="49">
+      <c r="AO112" s="47">
         <f>AU99</f>
         <v>9039000000</v>
       </c>
     </row>
     <row r="113" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN113" s="48" t="s">
+      <c r="AN113" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="AO113" s="49">
+      <c r="AO113" s="47">
         <f>AO110+AO111-AO112</f>
-        <v>92424289904.14418</v>
+        <v>146527384699.57388</v>
       </c>
     </row>
     <row r="114" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN114" s="48" t="s">
+      <c r="AN114" s="46" t="s">
         <v>155</v>
       </c>
-      <c r="AO114" s="50">
+      <c r="AO114" s="48">
         <f>AM34*(1+(5*AS16))</f>
         <v>448597263.29333401</v>
       </c>
     </row>
     <row r="115" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN115" s="51" t="s">
+      <c r="AN115" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="AO115" s="52">
+      <c r="AO115" s="50">
         <f>AO113/AO114</f>
-        <v>206.02954468696504</v>
+        <v>326.63459340758584</v>
       </c>
     </row>
     <row r="116" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN116" s="48" t="s">
+      <c r="AN116" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="AO116" s="64" cm="1">
+      <c r="AO116" s="56" cm="1">
         <f t="array" ref="AO116">_FV(A1,"Price",TRUE)</f>
-        <v>500.79</v>
+        <v>511.56</v>
       </c>
     </row>
     <row r="117" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN117" s="53" t="s">
+      <c r="AN117" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="AO117" s="54">
+      <c r="AO117" s="52">
         <f>AO115/AO116-1</f>
-        <v>-0.58859093694569575</v>
+        <v>-0.36149309287750053</v>
       </c>
     </row>
     <row r="118" spans="40:41" ht="20" x14ac:dyDescent="0.25">
-      <c r="AN118" s="53" t="s">
+      <c r="AN118" s="51" t="s">
         <v>159</v>
       </c>
-      <c r="AO118" s="55" t="str">
+      <c r="AO118" s="53" t="str">
         <f>IF(AO115&gt;AO116,"BUY","SELL")</f>
         <v>SELL</v>
       </c>

</xml_diff>